<commit_message>
feat(Marketing - Campañas): Agregadas variables a la importación de los contactos
</commit_message>
<xml_diff>
--- a/archivos/plantillas/marketing_importacion_campanias_contactos.xlsx
+++ b/archivos/plantillas/marketing_importacion_campanias_contactos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ecommerce\archivos\plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\simon_bolivar\ecommerce\archivos\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875AB6FF-74AA-4C62-A7FF-832C64B36969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D919C8CD-0351-4787-A66D-DC00D01DD258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8ADAB593-72DA-4AED-8D36-AA0FAA89A16B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8ADAB593-72DA-4AED-8D36-AA0FAA89A16B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Variable 1</t>
+  </si>
+  <si>
+    <t>Variable 2</t>
+  </si>
+  <si>
+    <t>Variable 3</t>
+  </si>
+  <si>
+    <t>Variable 4</t>
+  </si>
+  <si>
+    <t>Variable 5</t>
+  </si>
+  <si>
+    <t>Variable 6</t>
+  </si>
   <si>
     <t>NIT</t>
   </si>
@@ -99,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -109,9 +127,6 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,31 +442,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5ED38-F96E-4CC7-A802-43EAA271DABC}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="13.5546875" style="1"/>
+    <col min="1" max="1" width="27.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="33.6640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="13.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>

</xml_diff>